<commit_message>
Releasing successfully all COM Objects
</commit_message>
<xml_diff>
--- a/lib/MyExcel.xlsx
+++ b/lib/MyExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\source\repos\myexcel\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309C493C-B57F-414B-AAB8-76C1BFE77136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84D6D81-9968-437B-8E87-6620B284928E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>MyExcel</t>
+    <t>My Excel</t>
   </si>
 </sst>
 </file>

</xml_diff>